<commit_message>
rr Sat Nov  8 11:50:20 AM CET 2025
</commit_message>
<xml_diff>
--- a/public/routers/A8_Estudio/A81_Simplificado/A811_VIABILIDAD_ECONÓMICA_DE_LA_INVERSIÓN.xlsx
+++ b/public/routers/A8_Estudio/A81_Simplificado/A811_VIABILIDAD_ECONÓMICA_DE_LA_INVERSIÓN.xlsx
@@ -8,7 +8,6 @@
   </bookViews>
   <sheets>
     <sheet name="Parametros" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Coordenadas" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -544,55 +543,4 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Parámetro</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Valor</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>lat</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>lng</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>-4</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
 </file>
</xml_diff>